<commit_message>
Added a new JMeter scripts and list of scenarios
Added a new JMeter scripts and list of scenarios
</commit_message>
<xml_diff>
--- a/photov/Scenarios/Scenarios.xlsx
+++ b/photov/Scenarios/Scenarios.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Sr.No.</t>
   </si>
@@ -46,7 +46,13 @@
 Insert Message</t>
   </si>
   <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
     <t>Insert Place
+Insert Country
+Insert State
 Place List</t>
   </si>
 </sst>
@@ -85,7 +91,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -108,15 +114,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -413,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -473,11 +492,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="28.8">
+    <row r="7" spans="1:2" ht="57.6">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="28.8">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>